<commit_message>
part 2 + report finished
</commit_message>
<xml_diff>
--- a/doc/report/First&Follow_Table.xlsx
+++ b/doc/report/First&Follow_Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loicbermudez/Documents/ULB_PROJECT/Project-INFOF403-part2/more/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loicbermudez/Documents/ULB_PROJECT/Project-INFOF403-part2/doc/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECDD38B-377F-4A4F-AF6D-B1CDA7F738B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0978B280-161C-7C49-A5DC-C79454BCD323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{627F729E-ECEB-BF43-ABEE-9FAA9F5BEC1D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
   <si>
     <t>Non Terminal Symbols</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Cond</t>
   </si>
   <si>
-    <t>CondF</t>
-  </si>
-  <si>
     <t>ExprArith</t>
   </si>
   <si>
@@ -208,6 +205,45 @@
   </si>
   <si>
     <t>",", ), *, /, +, -, =, &gt;, &lt;, END, ELSE</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Vi</t>
+  </si>
+  <si>
+    <t>{∅}</t>
+  </si>
+  <si>
+    <t>{Code, ExprArith, Op, Comp, Print, Read}</t>
+  </si>
+  <si>
+    <t>{Code, ExprArith, Op, Comp, Print, Read, Program, Instruction, Assign, Cond}</t>
+  </si>
+  <si>
+    <t>{Code, ExprArith, Op, Comp, Print, Read, Program, Instruction, Assign, Cond, If, While}</t>
+  </si>
+  <si>
+    <t>{Program}</t>
+  </si>
+  <si>
+    <t>{Program, Code}</t>
+  </si>
+  <si>
+    <t>{Program, Code, Instruction}</t>
+  </si>
+  <si>
+    <t>{Program, Code, Instruction, Assign, If, While, Print, Read}</t>
+  </si>
+  <si>
+    <t>{Program, Code, Instruction, Assign, If, While, Print, Read, ExprArith, Cond}</t>
+  </si>
+  <si>
+    <t>{Program, Code, Instruction, Assign, If, While, Print, Read, ExprArith, Cond, Op, Comp}</t>
+  </si>
+  <si>
+    <t>Comp</t>
   </si>
 </sst>
 </file>
@@ -231,7 +267,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -463,11 +499,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -525,6 +579,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -843,7 +909,7 @@
   <dimension ref="B3:AC22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -884,79 +950,79 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="X4" s="2" t="s">
+      <c r="Y4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="Y4" s="2" t="s">
+      <c r="Z4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="Z4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AB4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AC4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.2">
@@ -964,10 +1030,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>2</v>
@@ -1003,10 +1069,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>3</v>
@@ -1054,10 +1120,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>4</v>
@@ -1097,10 +1163,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>5</v>
@@ -1141,16 +1207,16 @@
     </row>
     <row r="9" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="18"/>
@@ -1183,10 +1249,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>6</v>
@@ -1222,10 +1288,10 @@
         <v>7</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>7</v>
@@ -1263,10 +1329,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>8</v>
@@ -1302,10 +1368,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>9</v>
@@ -1344,16 +1410,16 @@
     </row>
     <row r="14" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="18"/>
@@ -1387,16 +1453,16 @@
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="18"/>
@@ -1432,16 +1498,16 @@
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="18"/>
@@ -1487,16 +1553,16 @@
     </row>
     <row r="17" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="18"/>
@@ -1532,16 +1598,16 @@
     </row>
     <row r="18" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="18"/>
@@ -1591,16 +1657,16 @@
     </row>
     <row r="19" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="18"/>
@@ -1636,16 +1702,16 @@
     </row>
     <row r="20" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="18"/>
@@ -1675,16 +1741,16 @@
     </row>
     <row r="21" spans="2:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="D21" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="19"/>
@@ -1722,20 +1788,115 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F8CF16-20AE-B846-BE0A-5C66219A4D3B}">
-  <dimension ref="B6"/>
+  <dimension ref="B6:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="68.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C7" s="20">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C8" s="20">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C9" s="20">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C10" s="22">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C16" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="22">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="22">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="22">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C20" s="22">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="22">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="22">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>